<commit_message>
push niet werkend sean(Walter)
</commit_message>
<xml_diff>
--- a/Uitslagen.xlsx
+++ b/Uitslagen.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +483,62 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>FICT</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SE</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>